<commit_message>
toản nộp bài tập buổi 3
</commit_message>
<xml_diff>
--- a/TestCase_Swag.xlsx
+++ b/TestCase_Swag.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AuToMaTionTes\baitap\ontap3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7056" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -151,14 +151,6 @@
 2.Click sản phẩm Sauce Labs Backpack</t>
   </si>
   <si>
-    <t>2.Verify trang chi tiết sản phẩm hiển thị đầy đủ:
-- tên sản phẩm
-- mô tả
-- giá
-- button add to cart
-- image</t>
-  </si>
-  <si>
     <t>1.Đăng nhập vào hệ thống
 2.Click add to cart sản phẩm Sauce Labs Bike Light</t>
   </si>
@@ -205,12 +197,40 @@
 - hiển thị đúng sản phẩm đã thêm ở ngoài trang chủ
 </t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.Verify trang chi tiết sản phẩm hiển thị đầy đủ:
+- tên sản phẩm
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Myriad Pro"/>
+        <charset val="163"/>
+      </rPr>
+      <t>- mô tả
+- giá</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Myriad Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- button add to cart
+- image</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +248,12 @@
       <color rgb="FFFF0000"/>
       <name val="Myriad Pro"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Myriad Pro"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="4">
@@ -277,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -298,6 +324,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,16 +613,16 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="22.19921875" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.4140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.08203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -620,7 +649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="55.2">
+    <row r="2" spans="1:7" ht="56">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -643,7 +672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="55.2">
+    <row r="3" spans="1:7" ht="56">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -666,7 +695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="55.2">
+    <row r="4" spans="1:7" ht="56">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -790,20 +819,20 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="24.09765625" customWidth="1"/>
+    <col min="2" max="2" width="24.08203125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="35.5" customWidth="1"/>
-    <col min="5" max="5" width="25.8984375" customWidth="1"/>
-    <col min="6" max="6" width="16.59765625" customWidth="1"/>
-    <col min="7" max="7" width="14.3984375" customWidth="1"/>
+    <col min="5" max="5" width="25.9140625" customWidth="1"/>
+    <col min="6" max="6" width="16.58203125" customWidth="1"/>
+    <col min="7" max="7" width="14.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.2" customHeight="1">
+    <row r="1" spans="1:7" ht="22.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -826,7 +855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="34.200000000000003" customHeight="1">
+    <row r="2" spans="1:7" ht="34.25" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -849,7 +878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="41.4">
+    <row r="3" spans="1:7" ht="42">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -872,7 +901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="41.4">
+    <row r="4" spans="1:7" ht="42">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -895,8 +924,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="96.6">
-      <c r="A5" s="3">
+    <row r="5" spans="1:7" ht="98">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -909,7 +938,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>10</v>
@@ -920,6 +949,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -931,12 +961,12 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="24.69921875" customWidth="1"/>
-    <col min="4" max="4" width="24.3984375" customWidth="1"/>
-    <col min="5" max="5" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.4140625" customWidth="1"/>
+    <col min="5" max="5" width="36.4140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="14.5" customWidth="1"/>
   </cols>
@@ -964,21 +994,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="55.2">
+    <row r="2" spans="1:7" ht="56">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>10</v>
@@ -987,21 +1017,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="110.4">
+    <row r="3" spans="1:7" ht="112">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>10</v>
@@ -1010,21 +1040,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="110.4">
+    <row r="4" spans="1:7" ht="112">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>10</v>

</xml_diff>